<commit_message>
Fix raw data, move investigations to main repo
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a_place_for_salvador_allende_raw.xlsx
+++ b/a-place-for-salvador-allende/a_place_for_salvador_allende_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\datasets-of-interest\a-place-for-salvador-allende\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A5D46F-AD7A-4856-9A53-82DB579ABAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D880C955-1F46-4B2A-ABB5-7D00F86C7F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14178,10 +14178,10 @@
   <dimension ref="A1:AO781"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18762,7 +18762,7 @@
         <v>-38.414416818917402</v>
       </c>
       <c r="M67" s="2">
-        <v>72.774796155920399</v>
+        <v>-72.774796155920399</v>
       </c>
       <c r="N67" s="2">
         <v>2010</v>

</xml_diff>